<commit_message>
Updated data after QA/QC
</commit_message>
<xml_diff>
--- a/data/raw_data/Owl_Species_Table.xlsx
+++ b/data/raw_data/Owl_Species_Table.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Owl_Species_Table"/>
   </sheets>
   <definedNames>
-    <definedName name="Owl_Species_Table">'Owl_Species_Table'!$A$1:$B$7</definedName>
+    <definedName name="Owl_Species_Table">'Owl_Species_Table'!$A$1:$B$12</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -383,55 +383,115 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Ferruginous Pygmy Owl</t>
+          <t>Ferruginous Pygmy-owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>GrHor</t>
+          <t>Fulvous</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Great Horned Owl</t>
+          <t>Guatamalan Barred Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Mottd</t>
+          <t>GrHor</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Mottled Owl</t>
+          <t>Great Horned Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>PacSc</t>
+          <t>Mottd</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Pacific Screech Owl</t>
+          <t>Mottled Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
+          <t>NoID</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Unidentified</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>PacSc</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Pacific Screech-owl</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
           <t>Specd</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>Spectacled Owl</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Styg</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Stygian Owl</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Whisk</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Whiskered Screech-owl</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data with corrected broadcast surveys
</commit_message>
<xml_diff>
--- a/data/raw_data/Owl_Species_Table.xlsx
+++ b/data/raw_data/Owl_Species_Table.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Owl_Species_Table"/>
   </sheets>
-  <definedNames>
-    <definedName name="Owl_Species_Table">'Owl_Species_Table'!$A$1:$B$12</definedName>
-  </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -26,6 +23,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000" tint="0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -33,6 +51,30 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,12 +85,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0D7E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0D7E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD0D7E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0D7E5"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFill="1" applyProtection="1" applyAlignment="1" applyFont="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="left"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="center"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
+      <alignment wrapText="1" vertical="center" horizontal="general"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,146 +442,150 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" min="1" max="1" width="16.2578125"/>
+    <col customWidth="true" min="2" max="2" width="30.61328125"/>
+  </cols>
   <sheetData>
     <row outlineLevel="0" r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Owl_Species_ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Owl_Species_Common_Name</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="2">
-      <c r="A2" s="0" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Barn</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Barn Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="3">
-      <c r="A3" s="0" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>FerPy</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>Ferruginous Pygmy-owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="4">
-      <c r="A4" s="0" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Fulvous</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Guatamalan Barred Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="5">
-      <c r="A5" s="0" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>GrHor</t>
         </is>
       </c>
-      <c r="B5" s="0" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Great Horned Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="6">
-      <c r="A6" s="0" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Mottd</t>
         </is>
       </c>
-      <c r="B6" s="0" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>Mottled Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="7">
-      <c r="A7" s="0" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>NoID</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Unidentified</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="8">
-      <c r="A8" s="0" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="B8" s="0" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="9">
-      <c r="A9" s="0" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>PacSc</t>
         </is>
       </c>
-      <c r="B9" s="0" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>Pacific Screech-owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="10">
-      <c r="A10" s="0" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Specd</t>
         </is>
       </c>
-      <c r="B10" s="0" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Spectacled Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="11">
-      <c r="A11" s="0" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Styg</t>
         </is>
       </c>
-      <c r="B11" s="0" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>Stygian Owl</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="12">
-      <c r="A12" s="0" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Whisk</t>
         </is>
       </c>
-      <c r="B12" s="0" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr">
         <is>
           <t>Whiskered Screech-owl</t>
         </is>

</xml_diff>